<commit_message>
Pruebas individuales Ivan Sprint 5
</commit_message>
<xml_diff>
--- a/Sprint#5/pruebas individuales Ivan/Log pruebas individuales RF-23.xlsx
+++ b/Sprint#5/pruebas individuales Ivan/Log pruebas individuales RF-23.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Oscar\Documents\GitHub\SIGAB\SIGAB\Sprint#5\pruebas individuales Oscar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivane\OneDrive\Escritorio\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B468F7-B230-4F60-9BAF-420D4230D888}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="RF 20" sheetId="1" r:id="rId1"/>
-    <sheet name="Firma" sheetId="6" r:id="rId2"/>
-    <sheet name="Firmas" sheetId="5" state="hidden" r:id="rId3"/>
+    <sheet name="RF 23" sheetId="1" r:id="rId1"/>
+    <sheet name="Datos de pruebas" sheetId="6" r:id="rId2"/>
+    <sheet name="Firma" sheetId="7" r:id="rId3"/>
+    <sheet name="Firmas" sheetId="5" state="hidden" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="105">
   <si>
     <t>Observación</t>
   </si>
@@ -62,6 +64,9 @@
   </si>
   <si>
     <t>Sí cumple</t>
+  </si>
+  <si>
+    <t>Jenny Ulate Montero</t>
   </si>
   <si>
     <t xml:space="preserve">Sistema de información para la gestión administrativa,
@@ -78,38 +83,303 @@
     <t>X</t>
   </si>
   <si>
-    <t>Plan gesti[on de redes sociales Ebdi (PDF)</t>
-  </si>
-  <si>
-    <t>Ejemplo asistencia Conferencia (PDF)</t>
-  </si>
-  <si>
-    <t>Cuadro Informe Redes Sociales (PDF)</t>
-  </si>
-  <si>
-    <t>Imágen de evidencia de actividad realizada por la EBDI (Imágen)</t>
-  </si>
-  <si>
-    <t>Taller Portafolio Bibliotecas (PDF)</t>
-  </si>
-  <si>
-    <t>Datos pruebas actividades (EXCEL)</t>
-  </si>
-  <si>
-    <t>Oscar Alvarado Gutiérrez</t>
-  </si>
-  <si>
-    <t>Autorizar una actividad interna.</t>
+    <t xml:space="preserve">RF-23 </t>
+  </si>
+  <si>
+    <t>Autorizar una actividad interna</t>
   </si>
   <si>
     <t>La verificación es brindada únicamente por un usuario autorizado de la administración</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los datos de prueba suministrados están en la otra hoja </t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tipo de actividad </t>
+  </si>
+  <si>
+    <t>Estado de la actividad (En ejecución, En progreso, Ejecutada)</t>
+  </si>
+  <si>
+    <t>Responsable de la actividad</t>
+  </si>
+  <si>
+    <t>Lugar donde se llevó a cabo la actividad</t>
+  </si>
+  <si>
+    <t>Recursos</t>
+  </si>
+  <si>
+    <t>Descripción de la actividad</t>
+  </si>
+  <si>
+    <t>Ejecutada</t>
+  </si>
+  <si>
+    <t>Juan Pablo Corella Parajales</t>
+  </si>
+  <si>
+    <t>Proposito de la actividad (capacitación, actualización, inducción. Involucramiento del personal, otro (s))</t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>Duración</t>
+  </si>
+  <si>
+    <t>Certificación de la actividad (participación o aprovechamiento)</t>
+  </si>
+  <si>
+    <t>Tema de la actividad</t>
+  </si>
+  <si>
+    <t>Responsable de coordinar actividad</t>
+  </si>
+  <si>
+    <t>Objetivos de la actividad</t>
+  </si>
+  <si>
+    <t>Agenda (Temas a tratar)</t>
+  </si>
+  <si>
+    <t>Ámbito (internacional o nacional)</t>
+  </si>
+  <si>
+    <t>Público dirigido (estudiantes regulares, graduados, docentes, administrativos)</t>
+  </si>
+  <si>
+    <t>Evaluación</t>
+  </si>
+  <si>
+    <t>Otro</t>
+  </si>
+  <si>
+    <t>Actividad Co-Curricular</t>
+  </si>
+  <si>
+    <t>Sesión sincrónica mediante Zoom</t>
+  </si>
+  <si>
+    <t>2 horas</t>
+  </si>
+  <si>
+    <r>
+      <t>No aplica</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (*)</t>
+    </r>
+  </si>
+  <si>
+    <t>Estudio de la realidad nacional</t>
+  </si>
+  <si>
+    <t>Kattia Bermúdez León</t>
+  </si>
+  <si>
+    <t>Concientizar a los estudiantes para que reflexionen acerca de temas como el aborto terapéutico, niños, alcoholismo y discriminación social y cultural</t>
+  </si>
+  <si>
+    <t>Saludo y bienvenida; Instrucciones para participar de la actividad: Entrega de protocolo para participar en foro en el aula virtual; Espacio para preguntas y comentarios; Cierre</t>
+  </si>
+  <si>
+    <t>Nacional</t>
+  </si>
+  <si>
+    <t>Los estudiantes abordaron temas tales como: aborto terapéutico, niñez, las cárceles, el alcoholismo discriminación social y cultural. A partir de estos temas se logra una toma de conciencia entre la comunidad estudiantil y la necesidad de contribuir desde la bibliotecología. Participación de 25 estudiantes</t>
+  </si>
+  <si>
+    <t>Computadora; conexión a Internet; plataforma Zoom; Lecturas; Aula virtual institucional</t>
+  </si>
+  <si>
+    <t>Estudiantes regulares del curso Introducción a la Bibliotecología y Gestión de la Información (I ciclo 2019)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">No aplica </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(*)</t>
+    </r>
+  </si>
+  <si>
+    <t>Inducción</t>
+  </si>
+  <si>
+    <t>Facultad de Filosofía y Letras</t>
+  </si>
+  <si>
+    <t>Proceso de inducción a estudiantes de primer ingreso</t>
+  </si>
+  <si>
+    <t>Estudiantes de primer ingreso</t>
+  </si>
+  <si>
+    <t>Capacitación</t>
+  </si>
+  <si>
+    <t>Curso</t>
+  </si>
+  <si>
+    <t>07 y 09 de setiembre de 2020</t>
+  </si>
+  <si>
+    <t>6 horas</t>
+  </si>
+  <si>
+    <t>Curso/taller sobre Microsoft Teams</t>
+  </si>
+  <si>
+    <t>Karla Rodríguez Salas</t>
+  </si>
+  <si>
+    <t>Magally Campos Méndez</t>
+  </si>
+  <si>
+    <t>Tareas; Chat; Llamadas; Equipos</t>
+  </si>
+  <si>
+    <t>Capacitación al personal docente de la EBDI. Participación de 11 docentes.</t>
+  </si>
+  <si>
+    <t>Invitación; instructivo; computadora; plataforma Microsoft Teams; conexión a internet</t>
+  </si>
+  <si>
+    <t>Personal docente de la EBDI</t>
+  </si>
+  <si>
+    <t>19, 25 y 26 de febrero de 2021</t>
+  </si>
+  <si>
+    <t>10 horas</t>
+  </si>
+  <si>
+    <t>Taller: uso de herramientas tecnológicas para la docencia</t>
+  </si>
+  <si>
+    <t>Magally Campos Méndez
+Freddy Oviedo</t>
+  </si>
+  <si>
+    <t>Herramientas del aula virtual (Asistencia, Grupos, Wiki, Glosario, lección, taller, cuestionario, insertar audio y url)
+Google calendar y Sharepoint</t>
+  </si>
+  <si>
+    <t>02 de setiembre</t>
+  </si>
+  <si>
+    <t>3 horas</t>
+  </si>
+  <si>
+    <t>Curso Classroom para docentes</t>
+  </si>
+  <si>
+    <t>Contribuir al formatalecimiento de las competencias académicas con respecto al manejo de herramientas para mediar pedagogicamente con las TIC</t>
+  </si>
+  <si>
+    <t>Google Classroom</t>
+  </si>
+  <si>
+    <t>Capacitación al personal docente de la EBDI. Participación de 10 docentes.</t>
+  </si>
+  <si>
+    <t>Invitación; instructivo; computadora; plataforma Zoom; conexión a internet</t>
+  </si>
+  <si>
+    <t>Curso/taller</t>
+  </si>
+  <si>
+    <t>Aula tecnológiga (Facultad de Filosofía y Letras)</t>
+  </si>
+  <si>
+    <t>30 de setiembre y 01 de octubre</t>
+  </si>
+  <si>
+    <t>16 horas</t>
+  </si>
+  <si>
+    <t>Escritura académica con énfasis en artículos científicos</t>
+  </si>
+  <si>
+    <t>Johann Pirela Morillo</t>
+  </si>
+  <si>
+    <t>Módulo 1: Aspectos introducctorios
+Módulo 2: Sistemas de citación y elementos para evaluar artículos científicos</t>
+  </si>
+  <si>
+    <t>Capacitación de dos días al personal docente de la EBDI. Participación de 11 docentes.</t>
+  </si>
+  <si>
+    <t>Invitación; Presentaciones PowerPoint; computadora; conexión a internet; proyección multimedia</t>
+  </si>
+  <si>
+    <t>Charla</t>
+  </si>
+  <si>
+    <t>17 de abril de 2018</t>
+  </si>
+  <si>
+    <t>Capacitación sobre las bases de datos del SIDUNA, el OPAC, libros y revistas electrónicos y el repositorio institucional</t>
+  </si>
+  <si>
+    <t>Pedro Bustabad</t>
+  </si>
+  <si>
+    <t>Jorlenny Valerio</t>
+  </si>
+  <si>
+    <t>Cumplir con la directriz institucional para el uso de los recursos del SIDUNA y fortalecer las habilidades del estudiantado.</t>
+  </si>
+  <si>
+    <t>Curso/taller a estudiantes regulares, egresados y graduados de la EBDI. Participación 25 estudiantes</t>
+  </si>
+  <si>
+    <t>Estudiantes regulares, egresados y graduados</t>
+  </si>
+  <si>
+    <t>16 y 18 de abril de 2018</t>
+  </si>
+  <si>
+    <t>Charla sobre el Centro Regional de Información sobre Desastres para América Latina y el Caribe (CRID)</t>
+  </si>
+  <si>
+    <t>Giannina Ocampo Bermúdez
+Lucrecia Barboza Jiménez</t>
+  </si>
+  <si>
+    <t>Centro Regional de Información sobre Desastres para América Latina y el Caribe (CRID)</t>
+  </si>
+  <si>
+    <t>Fortalecer las habilidades del estudiantado.</t>
+  </si>
+  <si>
+    <t>Estudiantes regulares</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,14 +465,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
-      <i/>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -236,6 +519,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -283,12 +572,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -298,7 +584,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="12"/>
     </xf>
@@ -308,9 +593,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -318,6 +600,26 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="2"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -336,33 +638,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Cálculo" xfId="2" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -387,55 +667,170 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>630758</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>76609</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1">
+        <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A708F16F-7A7C-43B3-96D9-7956B2A00F35}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{675A93A3-3062-41EE-BF6E-77DE134A0F86}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
+      <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="11715750" cy="8648700"/>
+          <a:ext cx="15108758" cy="2934109"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>630758</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>10045</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88F27A80-D284-44EE-A1F8-DBA663257CD1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="2952750"/>
+          <a:ext cx="15108758" cy="3724795"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>554548</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>143427</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA41E877-4721-4B9C-8437-2F101D04AFDC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="6667500"/>
+          <a:ext cx="15032548" cy="3953427"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>583127</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>152820</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagen 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7656B12F-30EA-4DB1-BE43-7380DD928801}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="10668000"/>
+          <a:ext cx="15061127" cy="3010320"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -463,7 +858,7 @@
         <xdr:cNvPr id="2" name="Imagen 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{77B5A9F6-0714-411B-A079-BBA359F1F23B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77B5A9F6-0714-411B-A079-BBA359F1F23B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -805,11 +1200,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -817,216 +1212,169 @@
     <col min="1" max="1" width="64.28515625" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" customWidth="1"/>
-    <col min="5" max="5" width="47" customWidth="1"/>
+    <col min="5" max="5" width="86.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="3"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="1:6" ht="98.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="9" t="s">
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>18</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+    </row>
+    <row r="4" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="4">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-    </row>
-    <row r="4" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A4" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="5">
-        <v>4</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="11">
-        <v>30</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="3"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="10">
-        <v>44334</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="B7" s="8">
+        <v>44335</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="15" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="14" t="s">
+    <row r="11" spans="1:6" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="5"/>
+    </row>
+    <row r="12" spans="1:6" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="6"/>
-    </row>
-    <row r="12" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="28"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="31"/>
-    </row>
-    <row r="13" spans="1:6" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="6"/>
-    </row>
-    <row r="14" spans="1:6" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="6"/>
-    </row>
-    <row r="15" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="6"/>
-    </row>
-    <row r="16" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="23"/>
-      <c r="B16" s="32"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-    </row>
-    <row r="17" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="24"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="26"/>
-    </row>
-    <row r="18" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-    </row>
-    <row r="19" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-    </row>
-    <row r="20" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A20" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-    </row>
-    <row r="21" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A21" s="15" t="s">
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+    </row>
+    <row r="13" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-    </row>
-    <row r="22" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A22" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+    </row>
+    <row r="16" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+    </row>
+    <row r="17" spans="3:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1043,10 +1391,528 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77B3D29C-B015-4D22-82CB-C4C05B9BC370}">
+  <dimension ref="A1:R9"/>
+  <sheetViews>
+    <sheetView zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
+      <selection activeCell="V8" sqref="V8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.28515625" customWidth="1"/>
+    <col min="9" max="9" width="20" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" customWidth="1"/>
+    <col min="11" max="11" width="19.85546875" customWidth="1"/>
+    <col min="12" max="12" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.85546875" customWidth="1"/>
+    <col min="15" max="15" width="19.7109375" customWidth="1"/>
+    <col min="16" max="16" width="18.85546875" customWidth="1"/>
+    <col min="17" max="17" width="24" customWidth="1"/>
+    <col min="19" max="19" width="22.85546875" customWidth="1"/>
+    <col min="20" max="20" width="21" customWidth="1"/>
+    <col min="21" max="21" width="23.28515625" customWidth="1"/>
+    <col min="22" max="22" width="32.28515625" customWidth="1"/>
+    <col min="23" max="23" width="31.85546875" customWidth="1"/>
+    <col min="24" max="24" width="26.28515625" customWidth="1"/>
+    <col min="25" max="25" width="75" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="78.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="31" customWidth="1"/>
+    <col min="28" max="28" width="23.42578125" customWidth="1"/>
+    <col min="29" max="29" width="69.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="45.85546875" customWidth="1"/>
+    <col min="31" max="31" width="27.85546875" customWidth="1"/>
+    <col min="32" max="32" width="23" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="29.140625" customWidth="1"/>
+    <col min="34" max="34" width="20.28515625" customWidth="1"/>
+    <col min="35" max="35" width="24.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="180" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="O1" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="P1" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="R1" s="17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="256.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="18">
+        <v>43605</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="K2" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="M2" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="N2" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="O2" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="P2" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q2" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="R2" s="16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="57" x14ac:dyDescent="0.25">
+      <c r="A3" s="16"/>
+      <c r="B3" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="18">
+        <v>43515</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" s="16"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="O3" s="16"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="R3" s="16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="16"/>
+      <c r="B4" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="I4" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="J4" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="K4" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="N4" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="O4" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="P4" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q4" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="R4" s="16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="114" x14ac:dyDescent="0.25">
+      <c r="A5" s="16"/>
+      <c r="B5" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="J5" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="K5" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="N5" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="O5" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="R5" s="16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="128.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="16"/>
+      <c r="B6" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="I6" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="K6" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="L6" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="M6" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="N6" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="O6" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="P6" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q6" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="R6" s="16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="114" x14ac:dyDescent="0.25">
+      <c r="A7" s="16"/>
+      <c r="B7" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="I7" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="J7" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="K7" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="N7" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="O7" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="P7" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q7" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="R7" s="16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="114" x14ac:dyDescent="0.25">
+      <c r="A8" s="16"/>
+      <c r="B8" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="J8" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="K8" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="L8" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="O8" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="P8" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q8" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="R8" s="16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="114" x14ac:dyDescent="0.25">
+      <c r="A9" s="16"/>
+      <c r="B9" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="I9" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="J9" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="K9" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="L9" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="O9" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="R9" s="16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCF06F9A-D2ED-4A27-B172-9CE156AFB7B3}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -1055,8 +1921,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4262D60A-F85A-498F-A7E9-091199FE6900}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0"/>

</xml_diff>